<commit_message>
now works, and there is a UFT result as well, Res3
</commit_message>
<xml_diff>
--- a/uftone-ai-aos-desktop-and-app/Default.xlsx
+++ b/uftone-ai-aos-desktop-and-app/Default.xlsx
@@ -15,11 +15,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
   <si>
     <t>Browser</t>
   </si>
   <si>
+    <t>device_manufacturer</t>
+  </si>
+  <si>
     <t>CHROME</t>
   </si>
   <si>
@@ -38,9 +41,6 @@
     <t xml:space="preserve">ce08171898ee74520c7e </t>
   </si>
   <si>
-    <t>iOS</t>
-  </si>
-  <si>
     <t xml:space="preserve">4092766f53caf4fe63d3467435a65abd4eafb9fd </t>
   </si>
   <si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>com.Advantage.aShopping</t>
-  </si>
-  <si>
-    <t>iPhone 6s</t>
   </si>
   <si>
     <t>Chrome</t>
@@ -547,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -560,7 +557,8 @@
     <col min="3" max="3" width="39.3828125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.95703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.6015625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16382" width="9.078125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="18.6953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16382" width="9.078125" style="2" customWidth="1"/>
     <col min="16383" max="16383" width="36.85546875" style="2" customWidth="1"/>
     <col min="16384" max="16384" width="9.078125" style="2" customWidth="1"/>
   </cols>
@@ -570,7 +568,7 @@
         <v>0</v>
       </c>
       <c t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c t="s">
         <v>10</v>
@@ -579,47 +577,53 @@
         <v>11</v>
       </c>
       <c t="s">
+        <v>3</v>
+      </c>
+      <c t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
         <v>2</v>
       </c>
+      <c s="1"/>
+      <c s="1" t="s">
+        <v>8</v>
+      </c>
+      <c s="1"/>
+      <c s="1" t="s">
+        <v>5</v>
+      </c>
+      <c s="3"/>
     </row>
     <row>
       <c s="1"/>
       <c s="1" t="s">
-        <v>13</v>
-      </c>
-      <c s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c s="1" t="s">
         <v>7</v>
       </c>
-      <c s="3" t="s">
-        <v>4</v>
-      </c>
+      <c s="1" t="s">
+        <v>9</v>
+      </c>
+      <c s="1" t="s">
+        <v>12</v>
+      </c>
+      <c s="3"/>
     </row>
     <row>
+      <c s="1" t="s">
+        <v>2</v>
+      </c>
+      <c s="1" t="s">
+        <v>13</v>
+      </c>
       <c s="1"/>
       <c s="1" t="s">
-        <v>5</v>
-      </c>
-      <c s="1" t="s">
-        <v>6</v>
-      </c>
-      <c s="1" t="s">
-        <v>9</v>
-      </c>
-      <c s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1" t="s">
-        <v>14</v>
-      </c>
-      <c s="1"/>
+        <v>0</v>
+      </c>
       <c s="1"/>
       <c s="3"/>
     </row>

</xml_diff>